<commit_message>
nomenclature Excel file import working
</commit_message>
<xml_diff>
--- a/public/NomenclatureImportFileExample.xlsx
+++ b/public/NomenclatureImportFileExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://testuma-my.sharepoint.com/personal/2081220_student_uma_pt/Documents/Mestrado/2º Ano/Projetc files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25ADBF77-A0D9-4684-9985-F7510E10F1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{25ADBF77-A0D9-4684-9985-F7510E10F1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DB11C96-86F2-4E2B-A3A4-5683288FEB1C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{ACC408D2-F281-451E-BEA0-56B82EF63FDA}"/>
+    <workbookView xWindow="4320" yWindow="5475" windowWidth="28800" windowHeight="15345" xr2:uid="{ACC408D2-F281-451E-BEA0-56B82EF63FDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="121">
   <si>
     <t>Animalia Linnaeus, 1758</t>
   </si>
@@ -342,16 +342,79 @@
   </si>
   <si>
     <t>486HSDP2</t>
+  </si>
+  <si>
+    <t>bibliography_key2</t>
+  </si>
+  <si>
+    <t>bibliography_key3</t>
+  </si>
+  <si>
+    <t>bibliography_key4</t>
+  </si>
+  <si>
+    <t>bibliography_key5</t>
+  </si>
+  <si>
+    <t>bibliography_key6</t>
+  </si>
+  <si>
+    <t>bibliography_key7</t>
+  </si>
+  <si>
+    <t>bibliography_key8</t>
+  </si>
+  <si>
+    <t>bibliography_key9</t>
+  </si>
+  <si>
+    <t>bibliography_key10</t>
+  </si>
+  <si>
+    <t>bibliography_key11</t>
+  </si>
+  <si>
+    <t>bibliography_key12</t>
+  </si>
+  <si>
+    <t>bibliography_key13</t>
+  </si>
+  <si>
+    <t>bibliography_key14</t>
+  </si>
+  <si>
+    <t>bibliography_key15</t>
+  </si>
+  <si>
+    <t>bibliography_key16</t>
+  </si>
+  <si>
+    <t>bibliography_key17</t>
+  </si>
+  <si>
+    <t>bibliography_key18</t>
+  </si>
+  <si>
+    <t>bibliography_key19</t>
+  </si>
+  <si>
+    <t>bibliography_key20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -713,15 +776,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB30EF3-4B47-4B9F-8499-9D2A6A0807FB}">
-  <dimension ref="A1:AL22"/>
+  <dimension ref="A1:AK22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD25" sqref="AD25"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -777,64 +840,64 @@
         <v>75</v>
       </c>
       <c r="S1" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="T1" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="U1" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="V1" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="W1" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="X1" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
       <c r="Y1" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="Z1" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="AA1" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="AB1" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="AC1" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="AD1" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="AE1" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="AF1" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="AG1" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="AH1" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="AI1" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
       <c r="AJ1" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="AK1" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -943,11 +1006,8 @@
       <c r="AK2" t="s">
         <v>101</v>
       </c>
-      <c r="AL2" t="s">
-        <v>88</v>
-      </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1006,7 +1066,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1125,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1184,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1243,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1242,7 +1302,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1361,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1420,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1419,7 +1479,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1478,7 +1538,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1597,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1596,7 +1656,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1655,7 +1715,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1774,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2128,6 +2188,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>